<commit_message>
Do no use default for deployment, fix function params
</commit_message>
<xml_diff>
--- a/tests/fixtures/datasets/SS2/SS2.xlsx
+++ b/tests/fixtures/datasets/SS2/SS2.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/google_drive_EBI/hca_clones/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6741126A-E399-6240-959F-A52D8A0DF03F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA16004-8CEE-2B44-87A2-D55DC417A59F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4040" yWindow="7900" windowWidth="28800" windowHeight="16580" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
-    <sheet name="Contact" sheetId="2" r:id="rId2"/>
-    <sheet name="Publications" sheetId="3" r:id="rId3"/>
-    <sheet name="Funder" sheetId="4" r:id="rId4"/>
+    <sheet name="Project - Contributors" sheetId="2" r:id="rId2"/>
+    <sheet name="Project - Publications" sheetId="3" r:id="rId3"/>
+    <sheet name="Project - Funders" sheetId="4" r:id="rId4"/>
     <sheet name="Donor organism" sheetId="5" r:id="rId5"/>
     <sheet name="Specimen from organism" sheetId="6" r:id="rId6"/>
     <sheet name="Cell suspension" sheetId="7" r:id="rId7"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="715">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -676,48 +676,6 @@
     <t>donor_organism.weight_unit.ontology_label</t>
   </si>
   <si>
-    <t>DONOR_ORGANISM.TIMECOURSE.TIMECOURSE_VALUE (Required)</t>
-  </si>
-  <si>
-    <t>The numerical value in Timecourse unit associated with a time interval used in the experiment.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> For example: 2</t>
-  </si>
-  <si>
-    <t>donor_organism.timecourse.timecourse_value</t>
-  </si>
-  <si>
-    <t>DONOR_ORGANISM.TIMECOURSE.TIMECOURSE_UNIT.TEXT (Required)</t>
-  </si>
-  <si>
-    <t>donor_organism.timecourse.timecourse_unit.text</t>
-  </si>
-  <si>
-    <t>DONOR_ORGANISM.TIMECOURSE.TIMECOURSE_UNIT.ONTOLOGY</t>
-  </si>
-  <si>
-    <t>donor_organism.timecourse.timecourse_unit.ontology</t>
-  </si>
-  <si>
-    <t>DONOR_ORGANISM.TIMECOURSE.TIMECOURSE_UNIT.ONTOLOGY_LABEL</t>
-  </si>
-  <si>
-    <t>donor_organism.timecourse.timecourse_unit.ontology_label</t>
-  </si>
-  <si>
-    <t>DONOR_ORGANISM.TIMECOURSE.TIMECOURSE_RELEVANCE</t>
-  </si>
-  <si>
-    <t>Relevance of the Timecourse value/unit to the experiment.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> For example: Collection after tumor cells injected into the mammary gland.</t>
-  </si>
-  <si>
-    <t>donor_organism.timecourse.timecourse_relevance</t>
-  </si>
-  <si>
     <t>specimen_from_organism.biomaterial_core.biomaterial_id</t>
   </si>
   <si>
@@ -850,9 +808,6 @@
     <t xml:space="preserve"> For example: my_gross_image_file.jpg</t>
   </si>
   <si>
-    <t>specimen_from_organism.state_of_specimen.gross_image</t>
-  </si>
-  <si>
     <t>ISCHEMIC TEMPERATURE</t>
   </si>
   <si>
@@ -898,9 +853,6 @@
     <t xml:space="preserve"> For example: my_microscopic_image_file.jpg</t>
   </si>
   <si>
-    <t>specimen_from_organism.state_of_specimen.microscopic_image</t>
-  </si>
-  <si>
     <t>POST-MORTEM INTERVAL</t>
   </si>
   <si>
@@ -1252,9 +1204,6 @@
     <t>Accession must start with DRR, SRR, or ERR. For example: SRR0000000</t>
   </si>
   <si>
-    <t>sequence_file.insdc_run</t>
-  </si>
-  <si>
     <t>LIBRARY PREPARATION ID</t>
   </si>
   <si>
@@ -1333,21 +1282,12 @@
     <t>The name of a process type being used.</t>
   </si>
   <si>
-    <t>collection_protocol.collection_method.text</t>
-  </si>
-  <si>
     <t>COLLECTION_PROTOCOL.COLLECTION_METHOD.ONTOLOGY</t>
   </si>
   <si>
-    <t>collection_protocol.collection_method.ontology</t>
-  </si>
-  <si>
     <t>COLLECTION_PROTOCOL.COLLECTION_METHOD.ONTOLOGY_LABEL</t>
   </si>
   <si>
-    <t>collection_protocol.collection_method.ontology_label</t>
-  </si>
-  <si>
     <t>dissociation_protocol.protocol_core.protocol_id</t>
   </si>
   <si>
@@ -1369,21 +1309,12 @@
     <t>DISSOCIATION_PROTOCOL.DISSOCIATION_METHOD.TEXT (Required)</t>
   </si>
   <si>
-    <t>dissociation_protocol.dissociation_method.text</t>
-  </si>
-  <si>
     <t>DISSOCIATION_PROTOCOL.DISSOCIATION_METHOD.ONTOLOGY</t>
   </si>
   <si>
-    <t>dissociation_protocol.dissociation_method.ontology</t>
-  </si>
-  <si>
     <t>DISSOCIATION_PROTOCOL.DISSOCIATION_METHOD.ONTOLOGY_LABEL</t>
   </si>
   <si>
-    <t>dissociation_protocol.dissociation_method.ontology_label</t>
-  </si>
-  <si>
     <t>enrichment_protocol.protocol_core.protocol_id</t>
   </si>
   <si>
@@ -1558,21 +1489,12 @@
     <t>The name of a library construction approach being used.</t>
   </si>
   <si>
-    <t>library_preparation_protocol.library_construction_approach.text</t>
-  </si>
-  <si>
     <t>LIBRARY_PREPARATION_PROTOCOL.LIBRARY_CONSTRUCTION_APPROACH.ONTOLOGY</t>
   </si>
   <si>
-    <t>library_preparation_protocol.library_construction_approach.ontology</t>
-  </si>
-  <si>
     <t>LIBRARY_PREPARATION_PROTOCOL.LIBRARY_CONSTRUCTION_APPROACH.ONTOLOGY_LABEL</t>
   </si>
   <si>
-    <t>library_preparation_protocol.library_construction_approach.ontology_label</t>
-  </si>
-  <si>
     <t>RETAIL NAME</t>
   </si>
   <si>
@@ -1768,21 +1690,12 @@
     <t>The name of a sequencing approach being used.</t>
   </si>
   <si>
-    <t>sequencing_protocol.sequencing_approach.text</t>
-  </si>
-  <si>
     <t>SEQUENCING_PROTOCOL.SEQUENCING_APPROACH.ONTOLOGY</t>
   </si>
   <si>
-    <t>sequencing_protocol.sequencing_approach.ontology</t>
-  </si>
-  <si>
     <t>SEQUENCING_PROTOCOL.SEQUENCING_APPROACH.ONTOLOGY_LABEL</t>
   </si>
   <si>
-    <t>sequencing_protocol.sequencing_approach.ontology_label</t>
-  </si>
-  <si>
     <t>SS2 1 Cell Integration Test</t>
   </si>
   <si>
@@ -2219,6 +2132,51 @@
   </si>
   <si>
     <t>cell_suspension.estimated_cell_count</t>
+  </si>
+  <si>
+    <t>sequence_file.insdc_run_accessions</t>
+  </si>
+  <si>
+    <t>collection_protocol.method.text</t>
+  </si>
+  <si>
+    <t>collection_protocol.method.ontology</t>
+  </si>
+  <si>
+    <t>collection_protocol.method.ontology_label</t>
+  </si>
+  <si>
+    <t>dissociation_protocol.method.text</t>
+  </si>
+  <si>
+    <t>dissociation_protocol.method.ontology</t>
+  </si>
+  <si>
+    <t>dissociation_protocol.method.ontology_label</t>
+  </si>
+  <si>
+    <t>library_preparation_protocol.library_construction_method.text</t>
+  </si>
+  <si>
+    <t>library_preparation_protocol.library_construction_method.ontology</t>
+  </si>
+  <si>
+    <t>library_preparation_protocol.library_construction_method.ontology_label</t>
+  </si>
+  <si>
+    <t>sequencing_protocol.method.text</t>
+  </si>
+  <si>
+    <t>sequencing_protocol.method.ontology</t>
+  </si>
+  <si>
+    <t>sequencing_protocol.method.ontology_label</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.state_of_specimen.gross_images</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.state_of_specimen.microscopic_images</t>
   </si>
 </sst>
 </file>
@@ -2748,16 +2706,16 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>724</v>
+        <v>695</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>725</v>
+        <v>696</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>726</v>
+        <v>697</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>727</v>
+        <v>698</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2774,25 +2732,25 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>583</v>
+        <v>554</v>
       </c>
       <c r="B6" t="s">
-        <v>583</v>
+        <v>554</v>
       </c>
       <c r="C6" t="s">
-        <v>585</v>
+        <v>556</v>
       </c>
       <c r="D6" t="s">
-        <v>584</v>
+        <v>555</v>
       </c>
       <c r="F6" t="s">
-        <v>721</v>
+        <v>692</v>
       </c>
       <c r="G6" t="s">
-        <v>586</v>
+        <v>557</v>
       </c>
       <c r="H6" t="s">
-        <v>587</v>
+        <v>558</v>
       </c>
     </row>
   </sheetData>
@@ -2805,7 +2763,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A6"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2818,54 +2776,54 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>411</v>
+        <v>394</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>414</v>
+        <v>397</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>417</v>
+        <v>400</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>444</v>
+        <v>424</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>446</v>
+        <v>425</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>448</v>
+        <v>426</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>412</v>
+        <v>395</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>415</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>432</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>136</v>
@@ -2885,13 +2843,13 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>421</v>
+        <v>404</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>87</v>
@@ -2905,31 +2863,31 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>438</v>
+        <v>418</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>439</v>
+        <v>419</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>440</v>
+        <v>420</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>441</v>
+        <v>421</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>442</v>
+        <v>422</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>443</v>
+        <v>423</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>445</v>
+        <v>704</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>447</v>
+        <v>705</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>449</v>
+        <v>706</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2947,31 +2905,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>684</v>
+        <v>655</v>
       </c>
       <c r="B6" t="s">
-        <v>679</v>
+        <v>650</v>
       </c>
       <c r="C6" t="s">
-        <v>680</v>
+        <v>651</v>
       </c>
       <c r="D6" t="s">
-        <v>674</v>
+        <v>645</v>
       </c>
       <c r="E6" t="s">
-        <v>675</v>
+        <v>646</v>
       </c>
       <c r="F6" t="s">
-        <v>676</v>
+        <v>647</v>
       </c>
       <c r="G6" t="s">
-        <v>683</v>
+        <v>654</v>
       </c>
       <c r="H6" t="s">
-        <v>681</v>
+        <v>652</v>
       </c>
       <c r="I6" t="s">
-        <v>682</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -2983,7 +2941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:A6"/>
     </sheetView>
   </sheetViews>
@@ -2998,63 +2956,63 @@
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>411</v>
+        <v>394</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>414</v>
+        <v>397</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>417</v>
+        <v>400</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>456</v>
+        <v>433</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>458</v>
+        <v>435</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>460</v>
+        <v>437</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>462</v>
+        <v>439</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>466</v>
+        <v>443</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>470</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>412</v>
+        <v>395</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>415</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>432</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>136</v>
@@ -3063,13 +3021,13 @@
         <v>139</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>463</v>
+        <v>440</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>467</v>
+        <v>444</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>471</v>
+        <v>448</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="102" x14ac:dyDescent="0.2">
@@ -3083,13 +3041,13 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>421</v>
+        <v>404</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>87</v>
@@ -3101,51 +3059,51 @@
         <v>87</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>464</v>
+        <v>441</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>468</v>
+        <v>445</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>472</v>
+        <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>450</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>451</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>455</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>457</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>469</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3166,34 +3124,34 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>685</v>
+        <v>656</v>
       </c>
       <c r="B6" t="s">
-        <v>686</v>
+        <v>657</v>
       </c>
       <c r="C6" t="s">
-        <v>687</v>
+        <v>658</v>
       </c>
       <c r="D6" t="s">
-        <v>674</v>
+        <v>645</v>
       </c>
       <c r="E6" t="s">
-        <v>675</v>
+        <v>646</v>
       </c>
       <c r="F6" t="s">
-        <v>676</v>
+        <v>647</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>689</v>
+        <v>660</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>690</v>
+        <v>661</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>691</v>
+        <v>662</v>
       </c>
       <c r="J6" t="s">
-        <v>688</v>
+        <v>659</v>
       </c>
       <c r="K6">
         <v>70</v>
@@ -3211,8 +3169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AH4" sqref="AH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3232,135 +3190,135 @@
   <sheetData>
     <row r="1" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>411</v>
+        <v>394</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>414</v>
+        <v>397</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>417</v>
+        <v>400</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>480</v>
+        <v>457</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>484</v>
+        <v>461</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>506</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>525</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>412</v>
+        <v>395</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>415</v>
+        <v>398</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>420</v>
+        <v>403</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>481</v>
+        <v>458</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>485</v>
+        <v>462</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>488</v>
+        <v>465</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>492</v>
+        <v>469</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>496</v>
+        <v>473</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>136</v>
@@ -3369,10 +3327,10 @@
         <v>139</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>503</v>
+        <v>480</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>507</v>
+        <v>484</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>136</v>
@@ -3381,49 +3339,49 @@
         <v>139</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>514</v>
+        <v>488</v>
       </c>
       <c r="S2" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="AD2" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>526</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>514</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="68" x14ac:dyDescent="0.2">
@@ -3437,189 +3395,189 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>421</v>
+        <v>404</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>482</v>
+        <v>459</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>87</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="AD3" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="AF3" s="2" t="s">
         <v>527</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>535</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>535</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>475</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>476</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>479</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>483</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>486</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="N4" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>707</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="R4" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>494</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>501</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>508</v>
-      </c>
-      <c r="P4" s="3" t="s">
+      <c r="T4" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="W4" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="X4" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y4" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="AC4" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>524</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>528</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>532</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>536</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>537</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>539</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>540</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>541</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>542</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>546</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>550</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3660,84 +3618,84 @@
     </row>
     <row r="6" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>692</v>
+        <v>663</v>
       </c>
       <c r="B6" t="s">
-        <v>694</v>
+        <v>665</v>
       </c>
       <c r="C6" t="s">
-        <v>693</v>
+        <v>664</v>
       </c>
       <c r="D6" t="s">
-        <v>674</v>
+        <v>645</v>
       </c>
       <c r="E6" t="s">
-        <v>675</v>
+        <v>646</v>
       </c>
       <c r="F6" t="s">
-        <v>676</v>
+        <v>647</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>695</v>
+        <v>666</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>696</v>
+        <v>667</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>695</v>
+        <v>666</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>697</v>
+        <v>668</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>698</v>
+        <v>669</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>699</v>
+        <v>670</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>698</v>
+        <v>669</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>700</v>
+        <v>671</v>
       </c>
       <c r="S6">
         <v>20014279</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>701</v>
+        <v>672</v>
       </c>
       <c r="U6" t="s">
-        <v>702</v>
+        <v>673</v>
       </c>
       <c r="V6" s="7"/>
       <c r="W6" t="s">
-        <v>703</v>
+        <v>674</v>
       </c>
       <c r="X6" t="s">
-        <v>704</v>
+        <v>675</v>
       </c>
       <c r="Y6">
         <v>20014279</v>
       </c>
       <c r="Z6" t="s">
-        <v>701</v>
+        <v>672</v>
       </c>
       <c r="AA6" t="s">
-        <v>702</v>
+        <v>673</v>
       </c>
       <c r="AB6" s="5"/>
       <c r="AC6" t="s">
-        <v>703</v>
+        <v>674</v>
       </c>
       <c r="AD6" s="6" t="s">
-        <v>705</v>
+        <v>676</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>706</v>
+        <v>677</v>
       </c>
       <c r="AF6" s="3" t="s">
-        <v>707</v>
+        <v>678</v>
       </c>
     </row>
   </sheetData>
@@ -3749,8 +3707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A6"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3767,69 +3725,69 @@
   <sheetData>
     <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>411</v>
+        <v>394</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>414</v>
+        <v>397</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>417</v>
+        <v>400</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>561</v>
+        <v>535</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>564</v>
+        <v>538</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>566</v>
+        <v>540</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>568</v>
+        <v>542</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>572</v>
+        <v>546</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>576</v>
+        <v>550</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>579</v>
+        <v>552</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>581</v>
+        <v>553</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>412</v>
+        <v>395</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>415</v>
+        <v>398</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>420</v>
+        <v>403</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>562</v>
+        <v>536</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>136</v>
@@ -3838,13 +3796,13 @@
         <v>139</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>569</v>
+        <v>543</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>573</v>
+        <v>547</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>577</v>
+        <v>551</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>136</v>
@@ -3864,13 +3822,13 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>421</v>
+        <v>404</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>87</v>
@@ -3882,10 +3840,10 @@
         <v>87</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>570</v>
+        <v>544</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>574</v>
+        <v>548</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>87</v>
@@ -3899,46 +3857,46 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>555</v>
+        <v>529</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>556</v>
+        <v>530</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>557</v>
+        <v>531</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>558</v>
+        <v>532</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>559</v>
+        <v>533</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>560</v>
+        <v>534</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>563</v>
+        <v>537</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>565</v>
+        <v>539</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>567</v>
+        <v>541</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>571</v>
+        <v>545</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>575</v>
+        <v>549</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>578</v>
+        <v>710</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>580</v>
+        <v>711</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>582</v>
+        <v>712</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3961,46 +3919,46 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>668</v>
+        <v>639</v>
       </c>
       <c r="B6" t="s">
-        <v>708</v>
+        <v>679</v>
       </c>
       <c r="C6" t="s">
-        <v>709</v>
+        <v>680</v>
       </c>
       <c r="D6" t="s">
-        <v>674</v>
+        <v>645</v>
       </c>
       <c r="E6" t="s">
-        <v>675</v>
+        <v>646</v>
       </c>
       <c r="F6" t="s">
-        <v>676</v>
+        <v>647</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>710</v>
+        <v>681</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>711</v>
+        <v>682</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>710</v>
+        <v>681</v>
       </c>
       <c r="J6" t="s">
-        <v>712</v>
+        <v>683</v>
       </c>
       <c r="K6" t="s">
-        <v>601</v>
+        <v>572</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>713</v>
+        <v>684</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>714</v>
+        <v>685</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>713</v>
+        <v>684</v>
       </c>
     </row>
   </sheetData>
@@ -4167,66 +4125,66 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>588</v>
+        <v>559</v>
       </c>
       <c r="B6" t="s">
-        <v>590</v>
+        <v>561</v>
       </c>
       <c r="C6" t="s">
-        <v>592</v>
+        <v>563</v>
       </c>
       <c r="D6" t="s">
-        <v>595</v>
+        <v>566</v>
       </c>
       <c r="E6" t="s">
-        <v>596</v>
+        <v>567</v>
       </c>
       <c r="F6" t="s">
-        <v>598</v>
+        <v>569</v>
       </c>
       <c r="G6" t="s">
-        <v>600</v>
+        <v>571</v>
       </c>
       <c r="H6" t="s">
-        <v>601</v>
+        <v>572</v>
       </c>
       <c r="I6" t="s">
-        <v>603</v>
+        <v>574</v>
       </c>
       <c r="J6" t="s">
-        <v>605</v>
+        <v>576</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>589</v>
+        <v>560</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>591</v>
+        <v>562</v>
       </c>
       <c r="C7" t="s">
-        <v>593</v>
+        <v>564</v>
       </c>
       <c r="D7" t="s">
-        <v>594</v>
+        <v>565</v>
       </c>
       <c r="E7" t="s">
-        <v>597</v>
+        <v>568</v>
       </c>
       <c r="F7" t="s">
-        <v>599</v>
+        <v>570</v>
       </c>
       <c r="G7" t="s">
-        <v>600</v>
+        <v>571</v>
       </c>
       <c r="H7" t="s">
-        <v>602</v>
+        <v>573</v>
       </c>
       <c r="I7" t="s">
-        <v>604</v>
+        <v>575</v>
       </c>
       <c r="J7" t="s">
-        <v>605</v>
+        <v>576</v>
       </c>
     </row>
   </sheetData>
@@ -4329,19 +4287,19 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>606</v>
+        <v>577</v>
       </c>
       <c r="B6" t="s">
-        <v>607</v>
+        <v>578</v>
       </c>
       <c r="C6" t="s">
-        <v>608</v>
+        <v>579</v>
       </c>
       <c r="D6">
         <v>27565351</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>609</v>
+        <v>580</v>
       </c>
     </row>
   </sheetData>
@@ -4356,8 +4314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4406,7 +4364,7 @@
         <v>96</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>723</v>
+        <v>694</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4418,13 +4376,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>610</v>
+        <v>581</v>
       </c>
       <c r="B6" t="s">
-        <v>611</v>
+        <v>582</v>
       </c>
       <c r="C6" t="s">
-        <v>612</v>
+        <v>583</v>
       </c>
     </row>
   </sheetData>
@@ -4436,8 +4394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AR6"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6:AA6"/>
+    <sheetView topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AN1" sqref="AN1:AR1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4473,11 +4431,11 @@
     <col min="37" max="37" width="42.6640625" customWidth="1"/>
     <col min="38" max="38" width="35.6640625" customWidth="1"/>
     <col min="39" max="39" width="41.6640625" customWidth="1"/>
-    <col min="40" max="40" width="53.6640625" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="57.6640625" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="50.6640625" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="56.6640625" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="46.6640625" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="53.6640625" customWidth="1"/>
+    <col min="41" max="41" width="57.6640625" customWidth="1"/>
+    <col min="42" max="42" width="50.6640625" customWidth="1"/>
+    <col min="43" max="43" width="56.6640625" customWidth="1"/>
+    <col min="44" max="44" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4598,21 +4556,11 @@
       <c r="AM1" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="AN1" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>224</v>
-      </c>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
     </row>
     <row r="2" spans="1:44" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -4732,21 +4680,11 @@
       <c r="AM2" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="AN2" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>225</v>
-      </c>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
     </row>
     <row r="3" spans="1:44" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -4866,21 +4804,11 @@
       <c r="AM3" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="AN3" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="AO3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AP3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AQ3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AR3" s="2" t="s">
-        <v>226</v>
-      </c>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -5000,21 +4928,11 @@
       <c r="AM4" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="AN4" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="AQ4" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="AR4" s="3" t="s">
-        <v>227</v>
-      </c>
+      <c r="AN4" s="3"/>
+      <c r="AO4" s="3"/>
+      <c r="AP4" s="3"/>
+      <c r="AQ4" s="3"/>
+      <c r="AR4" s="3"/>
     </row>
     <row r="5" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -5066,121 +4984,121 @@
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>613</v>
+        <v>584</v>
       </c>
       <c r="B6" t="s">
-        <v>614</v>
+        <v>585</v>
       </c>
       <c r="C6" t="s">
-        <v>615</v>
+        <v>586</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
-        <v>616</v>
+        <v>587</v>
       </c>
       <c r="F6" t="s">
-        <v>619</v>
+        <v>590</v>
       </c>
       <c r="G6" t="s">
-        <v>617</v>
+        <v>588</v>
       </c>
       <c r="H6" t="s">
-        <v>618</v>
+        <v>589</v>
       </c>
       <c r="I6">
         <v>36.4</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>620</v>
+        <v>591</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>621</v>
+        <v>592</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>622</v>
+        <v>593</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>623</v>
+        <v>594</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>624</v>
+        <v>595</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>623</v>
+        <v>594</v>
       </c>
       <c r="P6" t="s">
-        <v>625</v>
+        <v>596</v>
       </c>
       <c r="Q6" t="s">
-        <v>625</v>
+        <v>596</v>
       </c>
       <c r="R6" t="s">
-        <v>626</v>
+        <v>597</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>627</v>
+        <v>598</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>628</v>
+        <v>599</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>627</v>
+        <v>598</v>
       </c>
       <c r="V6" t="s">
-        <v>629</v>
+        <v>600</v>
       </c>
       <c r="W6" t="s">
-        <v>630</v>
+        <v>601</v>
       </c>
       <c r="X6" t="s">
-        <v>629</v>
+        <v>600</v>
       </c>
       <c r="Y6" t="s">
-        <v>715</v>
+        <v>686</v>
       </c>
       <c r="Z6" t="s">
-        <v>716</v>
+        <v>687</v>
       </c>
       <c r="AA6" t="s">
-        <v>715</v>
+        <v>686</v>
       </c>
       <c r="AB6">
         <v>22</v>
       </c>
       <c r="AC6" t="s">
-        <v>631</v>
+        <v>602</v>
       </c>
       <c r="AD6" s="3" t="s">
-        <v>632</v>
+        <v>603</v>
       </c>
       <c r="AE6" t="s">
-        <v>633</v>
+        <v>604</v>
       </c>
       <c r="AF6">
         <v>160</v>
       </c>
       <c r="AG6" t="s">
-        <v>634</v>
+        <v>605</v>
       </c>
       <c r="AH6" t="s">
-        <v>635</v>
+        <v>606</v>
       </c>
       <c r="AI6" t="s">
-        <v>634</v>
+        <v>605</v>
       </c>
       <c r="AJ6">
         <v>127</v>
       </c>
       <c r="AK6" t="s">
-        <v>637</v>
+        <v>608</v>
       </c>
       <c r="AL6" s="3" t="s">
-        <v>636</v>
+        <v>607</v>
       </c>
       <c r="AM6" t="s">
-        <v>638</v>
+        <v>609</v>
       </c>
     </row>
   </sheetData>
@@ -5192,8 +5110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AK6"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AC6" sqref="AC6"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5245,85 +5163,85 @@
         <v>124</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>305</v>
-      </c>
       <c r="AH1" s="1" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:37" ht="136" x14ac:dyDescent="0.2">
@@ -5364,7 +5282,7 @@
         <v>175</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>139</v>
@@ -5373,7 +5291,7 @@
         <v>175</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>139</v>
@@ -5388,34 +5306,34 @@
         <v>139</v>
       </c>
       <c r="U2" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="W2" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="X2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="AB2" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>298</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>161</v>
@@ -5427,10 +5345,10 @@
         <v>139</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:37" ht="68" x14ac:dyDescent="0.2">
@@ -5495,35 +5413,35 @@
         <v>87</v>
       </c>
       <c r="U3" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="Y3" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="V3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="X3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="AB3" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="AA3" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>299</v>
-      </c>
       <c r="AE3" s="2" t="s">
         <v>87</v>
       </c>
@@ -5534,124 +5452,124 @@
         <v>87</v>
       </c>
       <c r="AH3" s="2" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="AK3" s="2"/>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="O4" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>257</v>
-      </c>
       <c r="S4" s="3" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="T4" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="X4" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="V4" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="X4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="AB4" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="AF4" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="AB4" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>304</v>
-      </c>
       <c r="AG4" s="3" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="AI4" s="3" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="AJ4" s="3" t="s">
         <v>102</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>413</v>
+        <v>396</v>
       </c>
     </row>
     <row r="5" spans="1:37" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5697,115 +5615,115 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>654</v>
+        <v>625</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>639</v>
+        <v>610</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>640</v>
+        <v>611</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
+        <v>587</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="G6" t="s">
+        <v>588</v>
+      </c>
+      <c r="H6" t="s">
+        <v>589</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="L6" t="s">
+        <v>612</v>
+      </c>
+      <c r="M6" t="s">
+        <v>613</v>
+      </c>
+      <c r="N6" t="s">
+        <v>612</v>
+      </c>
+      <c r="O6" t="s">
+        <v>688</v>
+      </c>
+      <c r="P6" t="s">
+        <v>689</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>688</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="U6" t="s">
+        <v>614</v>
+      </c>
+      <c r="V6" t="s">
+        <v>615</v>
+      </c>
+      <c r="W6" t="s">
         <v>616</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>619</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="X6" t="s">
         <v>617</v>
-      </c>
-      <c r="H6" t="s">
-        <v>618</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>623</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>624</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>623</v>
-      </c>
-      <c r="L6" t="s">
-        <v>641</v>
-      </c>
-      <c r="M6" t="s">
-        <v>642</v>
-      </c>
-      <c r="N6" t="s">
-        <v>641</v>
-      </c>
-      <c r="O6" t="s">
-        <v>717</v>
-      </c>
-      <c r="P6" t="s">
-        <v>718</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>717</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>715</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>716</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>715</v>
-      </c>
-      <c r="U6" t="s">
-        <v>643</v>
-      </c>
-      <c r="V6" t="s">
-        <v>644</v>
-      </c>
-      <c r="W6" t="s">
-        <v>645</v>
-      </c>
-      <c r="X6" t="s">
-        <v>646</v>
       </c>
       <c r="Y6">
         <v>7200</v>
       </c>
       <c r="Z6" t="s">
-        <v>647</v>
+        <v>618</v>
       </c>
       <c r="AA6" t="s">
-        <v>648</v>
+        <v>619</v>
       </c>
       <c r="AB6">
         <v>2400</v>
       </c>
       <c r="AC6" t="s">
-        <v>720</v>
+        <v>691</v>
       </c>
       <c r="AD6">
         <v>5</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>631</v>
+        <v>602</v>
       </c>
       <c r="AF6" s="3" t="s">
-        <v>632</v>
+        <v>603</v>
       </c>
       <c r="AG6" s="3" t="s">
-        <v>633</v>
+        <v>604</v>
       </c>
       <c r="AH6" t="s">
-        <v>649</v>
+        <v>620</v>
       </c>
       <c r="AI6" t="s">
-        <v>650</v>
+        <v>621</v>
       </c>
       <c r="AJ6" s="3" t="s">
-        <v>613</v>
+        <v>584</v>
       </c>
       <c r="AK6" s="3" t="s">
-        <v>671</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -5865,61 +5783,61 @@
         <v>124</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="T1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>373</v>
-      </c>
       <c r="AA1" s="1" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="119" x14ac:dyDescent="0.2">
@@ -5948,10 +5866,10 @@
         <v>125</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>197</v>
@@ -5963,16 +5881,16 @@
         <v>139</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>142</v>
@@ -5984,7 +5902,7 @@
         <v>139</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="V2" s="2" t="s">
         <v>136</v>
@@ -5993,16 +5911,16 @@
         <v>139</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="68" x14ac:dyDescent="0.2">
@@ -6031,10 +5949,10 @@
         <v>126</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>87</v>
@@ -6046,16 +5964,16 @@
         <v>87</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>87</v>
@@ -6076,108 +5994,108 @@
         <v>87</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="K4" s="3" t="s">
+      <c r="N4" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="M4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="R4" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="Y4" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="T4" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>728</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>372</v>
-      </c>
       <c r="Z4" s="3" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>438</v>
+        <v>418</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>450</v>
+        <v>427</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6216,73 +6134,73 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>651</v>
+        <v>622</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>652</v>
+        <v>623</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>653</v>
+        <v>624</v>
       </c>
       <c r="D6">
         <v>9606</v>
       </c>
       <c r="E6" t="s">
-        <v>616</v>
+        <v>587</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>619</v>
+        <v>590</v>
       </c>
       <c r="G6" t="s">
-        <v>617</v>
+        <v>588</v>
       </c>
       <c r="H6" t="s">
-        <v>618</v>
+        <v>589</v>
       </c>
       <c r="I6" t="s">
-        <v>655</v>
+        <v>626</v>
       </c>
       <c r="J6" t="s">
-        <v>656</v>
+        <v>627</v>
       </c>
       <c r="K6" t="s">
-        <v>657</v>
+        <v>628</v>
       </c>
       <c r="L6" t="s">
-        <v>658</v>
+        <v>629</v>
       </c>
       <c r="M6" t="s">
-        <v>657</v>
+        <v>628</v>
       </c>
       <c r="N6">
         <v>98.7</v>
       </c>
       <c r="O6" t="s">
-        <v>659</v>
+        <v>630</v>
       </c>
       <c r="P6" t="s">
-        <v>660</v>
+        <v>631</v>
       </c>
       <c r="Q6">
         <v>10</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>623</v>
+        <v>594</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>624</v>
+        <v>595</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>623</v>
+        <v>594</v>
       </c>
       <c r="U6" t="s">
-        <v>661</v>
+        <v>632</v>
       </c>
       <c r="V6" t="s">
-        <v>662</v>
+        <v>633</v>
       </c>
       <c r="W6" t="s">
-        <v>661</v>
+        <v>632</v>
       </c>
       <c r="X6">
         <v>1</v>
@@ -6291,19 +6209,19 @@
         <v>2217</v>
       </c>
       <c r="Z6" t="s">
-        <v>663</v>
+        <v>634</v>
       </c>
       <c r="AA6" t="s">
-        <v>719</v>
+        <v>690</v>
       </c>
       <c r="AB6" s="3" t="s">
-        <v>654</v>
+        <v>625</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>684</v>
+        <v>655</v>
       </c>
       <c r="AD6" s="3" t="s">
-        <v>685</v>
+        <v>656</v>
       </c>
     </row>
   </sheetData>
@@ -6316,7 +6234,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6327,54 +6245,54 @@
   <sheetData>
     <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>399</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>400</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>408</v>
+        <v>391</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="119" x14ac:dyDescent="0.2">
@@ -6382,63 +6300,63 @@
         <v>87</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>401</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>409</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>406</v>
+        <v>700</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>410</v>
+        <v>393</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>474</v>
+        <v>451</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>555</v>
+        <v>529</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>722</v>
+        <v>693</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6458,13 +6376,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>664</v>
+        <v>635</v>
       </c>
       <c r="B6" t="s">
-        <v>666</v>
+        <v>637</v>
       </c>
       <c r="D6" t="s">
-        <v>669</v>
+        <v>640</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -6473,16 +6391,16 @@
         <v>75</v>
       </c>
       <c r="G6" t="s">
-        <v>670</v>
+        <v>641</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>651</v>
+        <v>622</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>692</v>
+        <v>663</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>668</v>
+        <v>639</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -6490,13 +6408,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>665</v>
+        <v>636</v>
       </c>
       <c r="B7" t="s">
-        <v>666</v>
+        <v>637</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>667</v>
+        <v>638</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -6505,16 +6423,16 @@
         <v>75</v>
       </c>
       <c r="G7" t="s">
-        <v>670</v>
+        <v>641</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>651</v>
+        <v>622</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>692</v>
+        <v>663</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>668</v>
+        <v>639</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -6544,7 +6462,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A6"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6557,54 +6475,54 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>411</v>
+        <v>394</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>414</v>
+        <v>397</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>417</v>
+        <v>400</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>431</v>
+        <v>414</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>434</v>
+        <v>416</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>436</v>
+        <v>417</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>412</v>
+        <v>395</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>415</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>432</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>136</v>
@@ -6624,13 +6542,13 @@
         <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>421</v>
+        <v>404</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>87</v>
@@ -6642,33 +6560,33 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>426</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>430</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>433</v>
+        <v>701</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>435</v>
+        <v>702</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>437</v>
+        <v>703</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6686,31 +6604,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>671</v>
+        <v>642</v>
       </c>
       <c r="B6" t="s">
-        <v>672</v>
+        <v>643</v>
       </c>
       <c r="C6" t="s">
-        <v>673</v>
+        <v>644</v>
       </c>
       <c r="D6" t="s">
-        <v>674</v>
+        <v>645</v>
       </c>
       <c r="E6" t="s">
-        <v>675</v>
+        <v>646</v>
       </c>
       <c r="F6" t="s">
-        <v>676</v>
+        <v>647</v>
       </c>
       <c r="G6" t="s">
-        <v>677</v>
+        <v>648</v>
       </c>
       <c r="H6" t="s">
-        <v>678</v>
+        <v>649</v>
       </c>
       <c r="I6" t="s">
-        <v>677</v>
+        <v>648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>